<commit_message>
Enslaved Original Axioms Evaluation results
</commit_message>
<xml_diff>
--- a/Enslaved/Original/Axiomatization/Results/Enslaved_Axioms.txt_cq_GPT4o_results.xlsx
+++ b/Enslaved/Original/Axiomatization/Results/Enslaved_Axioms.txt_cq_GPT4o_results.xlsx
@@ -1,26 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10413"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chrisdavisj/graph-rag-iswc-2025/util-scripts/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F29A95F-4572-3840-BEBE-A258027B5C0D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
-  <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="29400" windowHeight="17120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
-  </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet state="visible" name="Sheet1" sheetId="1" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <definedNames/>
+  <calcPr/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="126">
   <si>
     <t>CQ</t>
   </si>
@@ -32,6 +23,12 @@
   </si>
   <si>
     <t>GPT4o_Raw</t>
+  </si>
+  <si>
+    <t>Score</t>
+  </si>
+  <si>
+    <t>Notes</t>
   </si>
   <si>
     <t>What are all the enslaved people in County X in the century X?</t>
@@ -47,7 +44,7 @@
 - Provide the full SPARQL query without placeholders.
 Context:
 Below is the schema of a knowledge graph:
-﻿not (&lt;https://enslaved.org/ontology/Person&gt;) SubClassOf not (&lt;https://enslaved.org/ontology/hasAgentRecord&gt; only 
+not (&lt;https://enslaved.org/ontology/Person&gt;) SubClassOf not (&lt;https://enslaved.org/ontology/hasAgentRecord&gt; only 
 (&lt;https://enslaved.org/ontology/AgeRecord&gt; or &lt;https://enslaved.org/ontology/OccupationRecord&gt; or &lt;https://enslaved.org/ontology/OriginRecord&gt; or &lt;https://enslaved.org/ontology/PersonStatusRecord&gt; or &lt;https://enslaved.org/ontology/RaceRecord&gt; or &lt;https://enslaved.org/ontology/SexRecord&gt;))
 &lt;https://enslaved.org/ontology/fallsWithin&gt; some &lt;https://enslaved.org/ontology/TimeSpan&gt; SubClassOf &lt;https://enslaved.org/ontology/TemporalExtent&gt;
 &lt;https://enslaved.org/ontology/generatedBy&gt; some &lt;https://enslaved.org/ontology/ProvenanceActivity&gt; SubClassOf &lt;https://enslaved.org/ontology/EntityWithProvenance&gt;
@@ -137,6 +134,12 @@
     },
     "error": null
 }</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - Valid SPARQL Query
+ - missed one entity and relation between entities (Event to Timespan - missing Temporal Extent) hop issue
+ - Hallucinated County class instead of Place
+ - if fixed, might adequately answer the CQ</t>
   </si>
   <si>
     <t>What are all the enslaved individuals categorized by gender, ethnicity, and location (e.g., on plantation X or of XXXX ethnicity)?</t>
@@ -235,6 +238,12 @@
 }</t>
   </si>
   <si>
+    <t xml:space="preserve"> - Almost valid Sparql
+ - out of the 3 classes it explores in optional, only one route is correct
+ - hallucinated the same relationship in all of the optional class exploration
+ - Needs a lot of change to make it work and adequately answer CQ</t>
+  </si>
+  <si>
     <t>What are all the available population counts of enslaved people by place and year?</t>
   </si>
   <si>
@@ -332,6 +341,11 @@
 }</t>
   </si>
   <si>
+    <t xml:space="preserve"> - Valid SPARQL syntax
+ - Invalid Entity to relationship tagging
+ - requires a lot of effort and schema compliance to even remotely answer the CQ</t>
+  </si>
+  <si>
     <t>What are all the documented literacy statuses of enslaved individuals?</t>
   </si>
   <si>
@@ -428,6 +442,10 @@
 }</t>
   </si>
   <si>
+    <t xml:space="preserve"> - Valid SPARQL syntax
+ - Everything has correct entity to relationship tags</t>
+  </si>
+  <si>
     <t>What are all the geographical places associated with enslaved people and their relationships to those places?</t>
   </si>
   <si>
@@ -523,6 +541,12 @@
 }</t>
   </si>
   <si>
+    <t xml:space="preserve"> - Valid SPARQL and retrieves data
+ - Common interpretation of Agent to Person
+ - Doesn't retrieve the valid place data
+ - with minimal changes, can adequately answer the CQ</t>
+  </si>
+  <si>
     <t>What are all the common names of enslaved children during the Revolutionary War era?</t>
   </si>
   <si>
@@ -629,6 +653,12 @@
 }</t>
   </si>
   <si>
+    <t xml:space="preserve"> - Valid SPARQL Query
+ - missed one entity and relation between entities (Event to Timespan - missing Temporal Extent) hop issue
+ - Hallucinated commonName relationship
+ - if fixed, might adequately answer the CQ</t>
+  </si>
+  <si>
     <t>What are all the enslaved individuals and who enslaved them, including locations?</t>
   </si>
   <si>
@@ -724,6 +754,12 @@
 }</t>
   </si>
   <si>
+    <t xml:space="preserve"> - Valid SPARQL Query
+ - minor Prefix issues
+ - location relationship issue from Person class
+ - otherwise, if fixed, can adequately answer the CQ and and probably answer part of the CQ even without location tagging</t>
+  </si>
+  <si>
     <t>Who are all the children associated with enslaved individuals?</t>
   </si>
   <si>
@@ -822,6 +858,13 @@
 }</t>
   </si>
   <si>
+    <t xml:space="preserve"> - Valid SPARQL
+ - Correctly Captures data
+ - returns child entities
+ - explores additional unused chains but still functions
+ - adequately answers the CQ</t>
+  </si>
+  <si>
     <t>What are all the available records about individuals identified as enslaved or formerly enslaved in specific locations and periods?</t>
   </si>
   <si>
@@ -924,6 +967,13 @@
 }</t>
   </si>
   <si>
+    <t xml:space="preserve"> - Valid SPARQL Query
+ - minor issues
+ - missing hop issue for temporal extent
+ - hallucinated location class
+ - otherwise, if fixed, can adequately answer the CQ and and probably answer part of the CQ even without location tagging</t>
+  </si>
+  <si>
     <t>What are all the enslaved children recorded in specific locations and time periods?</t>
   </si>
   <si>
@@ -1033,6 +1083,13 @@
 }</t>
   </si>
   <si>
+    <t xml:space="preserve"> - Valid SPARQL
+ - minor issues
+ - hop issues from Event to Temporal extent and Participant role
+ - minor relationship typos
+ - if corrected, can adequately answer the CQ</t>
+  </si>
+  <si>
     <t>What are all the enslaved people associated with a specific owner in a specific place and time, and how many were there?</t>
   </si>
   <si>
@@ -1133,6 +1190,14 @@
 }</t>
   </si>
   <si>
+    <t>- Valid SPARQL
+ - minor issues
+ - person to temporal extent hop issue 
+- location relationship issue from the Person class
+ - if fixed, can adequately answer the CQ
+ - didn't include specific filters or grouping for owners and place</t>
+  </si>
+  <si>
     <t>What are all the enslaved individuals who contributed labor to construction projects, such as the state capitol, and what were their roles?</t>
   </si>
   <si>
@@ -1231,6 +1296,11 @@
 }</t>
   </si>
   <si>
+    <t xml:space="preserve"> - Valid SPARQL
+ - minor missing hop or relationship issue from occupation to participant role type
+- if corrected, adequately answers CQ</t>
+  </si>
+  <si>
     <t>What are all the known addresses or properties that were inhabited by enslaved individuals?</t>
   </si>
   <si>
@@ -1329,6 +1399,11 @@
 }</t>
   </si>
   <si>
+    <t xml:space="preserve"> - Valid SPARQL
+ - Invalid  too many incorrect relationships and entities
+ - requires a lot of effort to correct and make it work to adequately answer the CQ</t>
+  </si>
+  <si>
     <t>What are all the enslaved individuals transported from specific ports and their demographic breakdowns over time?</t>
   </si>
   <si>
@@ -1435,6 +1510,14 @@
 }</t>
   </si>
   <si>
+    <t>- Valid SPARQL
+ - many minor issues
+ - Event to temporal extent hop issue 
+ - location relationship issue. Port misunderstood as Event
+ - agent record subclasses to age, race, and sex not resolved correctly for parameters, uses 'contains' relationship which does exist
+ - if fixed, can maybe answer the CQ</t>
+  </si>
+  <si>
     <t>What are all the known slave rebellions, their participants, locations, and dates?</t>
   </si>
   <si>
@@ -1533,6 +1616,12 @@
 }</t>
   </si>
   <si>
+    <t xml:space="preserve"> - Valid SPARQL
+ - The logic is correct but minor issues
+ - hop issues for temporal extent, participant role, and place
+ - if resolved, will adequately answer the CQ</t>
+  </si>
+  <si>
     <t>What are all the known relatives of enslaved individuals, including their relationships and locations?</t>
   </si>
   <si>
@@ -1632,6 +1721,11 @@
 }</t>
   </si>
   <si>
+    <t xml:space="preserve"> - Valid SPARQL query
+ - mostly correct except the location missing hop
+ - if fixed, will answer the CQ adequately </t>
+  </si>
+  <si>
     <t>What are all the median ages of enslaved individuals who escaped in location X during time period X?</t>
   </si>
   <si>
@@ -1741,6 +1835,14 @@
 }</t>
   </si>
   <si>
+    <t xml:space="preserve"> - Valid SPARQL
+ - lot of minor issues
+ - hop issues to temporal extent from event
+ - Location class and relationship hallucinated
+ - participant role relationship typo
+ - if fixed, will adequately answer the CQ</t>
+  </si>
+  <si>
     <t>What are all the average ages at death of enslaved individuals?</t>
   </si>
   <si>
@@ -1841,6 +1943,11 @@
 }</t>
   </si>
   <si>
+    <t xml:space="preserve"> - valid SPARQL
+ - hallucinated invalid relationship and aggregations on it
+ - will take effort and knowledge of schema to fix it to answer cq</t>
+  </si>
+  <si>
     <t>What are all the documented skill categories associated with enslaved individuals, broken down by ethnic group, and their percentages?</t>
   </si>
   <si>
@@ -1949,6 +2056,11 @@
 }</t>
   </si>
   <si>
+    <t xml:space="preserve"> - invalid SPARQL
+ - doesn't even traverse through correct relationships and perform aggregations in a way that is correctable
+ - requires a lot of effort and redo to answer the CQ</t>
+  </si>
+  <si>
     <t>What are all the recorded marriage events between enslaved individuals, categorized by same or different ethnic groupings, and their percentages?</t>
   </si>
   <si>
@@ -2059,6 +2171,11 @@
 }</t>
   </si>
   <si>
+    <t xml:space="preserve"> - minor approach fault causing invalid SPARQL - missing join
+ - minor relationship typos
+ - if fixed, can adequately answer CQ</t>
+  </si>
+  <si>
     <t>What are all the known economic values assigned to enslaved individuals, categorized by ethnicity, skills, gender, and period?</t>
   </si>
   <si>
@@ -2174,6 +2291,14 @@
 }</t>
   </si>
   <si>
+    <t xml:space="preserve"> - valid SPARQL
+ - a lot of minor issues
+ - hallucinated economic value entity and relationship
+ - invalid resolution of race, occupation, and sex records
+ - missing hop for temporal extent
+ - requires a lot of rework to fix the query</t>
+  </si>
+  <si>
     <t>What are all the life outcomes (e.g., sale, manumission, death) of enslaved individuals disembarked from ship XXX?</t>
   </si>
   <si>
@@ -2270,6 +2395,13 @@
 }</t>
   </si>
   <si>
+    <t xml:space="preserve"> - valid SPARQL
+ - minor issues
+ - mostly looks fine
+ - typo for role relationship/hop issue
+ - if fixed can answer the CQ</t>
+  </si>
+  <si>
     <t>What are all the enslaved individuals who lived in location X in the time period XXX?</t>
   </si>
   <si>
@@ -2372,6 +2504,13 @@
 }</t>
   </si>
   <si>
+    <t xml:space="preserve"> - valid SPARQL
+ - missing hop for temporal extent from event
+ - hallucinated location
+ - minor issues
+ - if fixed, can adequately answer CQ</t>
+  </si>
+  <si>
     <t>What are all the enslaved individuals who were later recorded as slave owners, including details of their ownership activities?</t>
   </si>
   <si>
@@ -2476,29 +2615,38 @@
 }</t>
   </si>
   <si>
-    <t>Score</t>
-  </si>
-  <si>
-    <t>Notes</t>
+    <t xml:space="preserve"> - valid SPARQL
+ - minor issues
+ - missing hop/resolution issue for ownership activity
+ - if fixed, can answer the CQ</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <fonts count="4">
     <font>
-      <sz val="11"/>
+      <sz val="11.0"/>
       <color theme="1"/>
       <name val="Calibri"/>
-      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="11"/>
+      <sz val="11.0"/>
+      <color theme="1"/>
       <name val="Calibri"/>
-      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11.0"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -2506,90 +2654,83 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="gray125"/>
+      <patternFill patternType="lightGray"/>
     </fill>
   </fills>
   <borders count="3">
+    <border/>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
     </border>
     <border>
       <left style="thin">
-        <color auto="1"/>
+        <color rgb="FF000000"/>
       </left>
       <right style="thin">
-        <color auto="1"/>
+        <color rgb="FF000000"/>
       </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="4">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
+  <cellXfs count="6">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    <xf borderId="2" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" shrinkToFit="0" vertical="top" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle xfId="0" name="Normal" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Sheets">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:srgbClr val="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:srgbClr val="FFFFFF"/>
       </a:lt1>
       <a:dk2>
-        <a:srgbClr val="1F497D"/>
+        <a:srgbClr val="000000"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="EEECE1"/>
+        <a:srgbClr val="FFFFFF"/>
       </a:lt2>
       <a:accent1>
         <a:srgbClr val="4F81BD"/>
@@ -2613,77 +2754,19 @@
         <a:srgbClr val="0000FF"/>
       </a:hlink>
       <a:folHlink>
-        <a:srgbClr val="800080"/>
+        <a:srgbClr val="0000FF"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Sheets">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
-        <a:ea typeface=""/>
-        <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Times New Roman"/>
-        <a:font script="Hebr" typeface="Times New Roman"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="MoolBoran"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Times New Roman"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:latin typeface="Calibri"/>
+        <a:ea typeface="Calibri"/>
+        <a:cs typeface="Calibri"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
-        <a:ea typeface=""/>
-        <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Arial"/>
-        <a:font script="Hebr" typeface="Arial"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="DaunPenh"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Arial"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:ea typeface="Calibri"/>
+        <a:cs typeface="Calibri"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -2695,185 +2778,154 @@
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:tint val="50000"/>
-                <a:satMod val="300000"/>
+                <a:lumMod val="110000"/>
+                <a:satMod val="105000"/>
+                <a:tint val="67000"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="35000">
+            <a:gs pos="50000">
               <a:schemeClr val="phClr">
-                <a:tint val="37000"/>
-                <a:satMod val="300000"/>
+                <a:lumMod val="105000"/>
+                <a:satMod val="103000"/>
+                <a:tint val="73000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:tint val="15000"/>
-                <a:satMod val="350000"/>
+                <a:lumMod val="105000"/>
+                <a:satMod val="109000"/>
+                <a:tint val="81000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="16200000" scaled="1"/>
+          <a:lin ang="5400000" scaled="0"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:shade val="51000"/>
-                <a:satMod val="130000"/>
+                <a:satMod val="103000"/>
+                <a:lumMod val="102000"/>
+                <a:tint val="94000"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="80000">
+            <a:gs pos="50000">
               <a:schemeClr val="phClr">
-                <a:shade val="93000"/>
-                <a:satMod val="130000"/>
+                <a:satMod val="110000"/>
+                <a:lumMod val="100000"/>
+                <a:shade val="100000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:shade val="94000"/>
-                <a:satMod val="135000"/>
+                <a:lumMod val="99000"/>
+                <a:satMod val="120000"/>
+                <a:shade val="78000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="16200000" scaled="0"/>
+          <a:lin ang="5400000" scaled="0"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr">
-              <a:shade val="95000"/>
-              <a:satMod val="105000"/>
-            </a:schemeClr>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-        </a:ln>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
         </a:ln>
       </a:lnStyleLst>
       <a:effectStyleLst>
         <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
               <a:srgbClr val="000000">
-                <a:alpha val="38000"/>
+                <a:alpha val="63000"/>
               </a:srgbClr>
             </a:outerShdw>
           </a:effectLst>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
-              <a:srgbClr val="000000">
-                <a:alpha val="35000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
-              <a:srgbClr val="000000">
-                <a:alpha val="35000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
-          <a:scene3d>
-            <a:camera prst="orthographicFront">
-              <a:rot lat="0" lon="0" rev="0"/>
-            </a:camera>
-            <a:lightRig rig="threePt" dir="t">
-              <a:rot lat="0" lon="0" rev="1200000"/>
-            </a:lightRig>
-          </a:scene3d>
-          <a:sp3d>
-            <a:bevelT w="63500" h="25400"/>
-          </a:sp3d>
         </a:effectStyle>
       </a:effectStyleLst>
       <a:bgFillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:tint val="95000"/>
+            <a:satMod val="170000"/>
+          </a:schemeClr>
+        </a:solidFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:tint val="40000"/>
-                <a:satMod val="350000"/>
+                <a:tint val="93000"/>
+                <a:satMod val="150000"/>
+                <a:shade val="98000"/>
+                <a:lumMod val="102000"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="40000">
+            <a:gs pos="50000">
               <a:schemeClr val="phClr">
-                <a:tint val="45000"/>
-                <a:shade val="99000"/>
-                <a:satMod val="350000"/>
+                <a:tint val="98000"/>
+                <a:satMod val="130000"/>
+                <a:shade val="90000"/>
+                <a:lumMod val="103000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:shade val="20000"/>
-                <a:satMod val="255000"/>
+                <a:shade val="63000"/>
+                <a:satMod val="120000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:path path="circle">
-            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
-          </a:path>
-        </a:gradFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:tint val="80000"/>
-                <a:satMod val="300000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:shade val="30000"/>
-                <a:satMod val="200000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:path path="circle">
-            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
-          </a:path>
+          <a:lin ang="5400000" scaled="0"/>
         </a:gradFill>
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
-  <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F25"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <pageSetUpPr/>
+  </sheetPr>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="4" width="62" style="2" customWidth="1"/>
-    <col min="5" max="5" width="12.6640625" style="2" customWidth="1"/>
-    <col min="6" max="6" width="49.83203125" style="2" customWidth="1"/>
+    <col customWidth="1" min="1" max="4" width="62.0"/>
+    <col customWidth="1" min="5" max="5" width="12.71"/>
+    <col customWidth="1" min="6" max="6" width="49.86"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2886,350 +2938,497 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" ht="375.0" customHeight="1">
+      <c r="A2" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" ht="375.0" customHeight="1">
+      <c r="A3" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" s="4">
+        <v>-1.0</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" ht="375.0" customHeight="1">
+      <c r="A4" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E4" s="4">
+        <v>-1.0</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" ht="375.0" customHeight="1">
+      <c r="A5" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E5" s="4">
+        <v>1.0</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="6" ht="375.0" customHeight="1">
+      <c r="A6" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="E6" s="4">
+        <v>0.0</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="7" ht="375.0" customHeight="1">
+      <c r="A7" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="E7" s="4">
+        <v>0.0</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="8" ht="375.0" customHeight="1">
+      <c r="A8" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="E8" s="4">
+        <v>0.0</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="9" ht="375.0" customHeight="1">
+      <c r="A9" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="E9" s="4">
+        <v>1.0</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="10" ht="375.0" customHeight="1">
+      <c r="A10" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="E10" s="4">
+        <v>0.0</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="11" ht="375.0" customHeight="1">
+      <c r="A11" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="E11" s="4">
+        <v>0.0</v>
+      </c>
+      <c r="F11" s="4" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="12" ht="375.0" customHeight="1">
+      <c r="A12" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="E12" s="4">
+        <v>-1.0</v>
+      </c>
+      <c r="F12" s="4" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="13" ht="375.0" customHeight="1">
+      <c r="A13" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="E13" s="4">
+        <v>0.0</v>
+      </c>
+      <c r="F13" s="4" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="14" ht="375.0" customHeight="1">
+      <c r="A14" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="E14" s="4">
+        <v>-1.0</v>
+      </c>
+      <c r="F14" s="4" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="15" ht="375.0" customHeight="1">
+      <c r="A15" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="E15" s="4">
+        <v>-1.0</v>
+      </c>
+      <c r="F15" s="4" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="16" ht="375.0" customHeight="1">
+      <c r="A16" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="E16" s="4">
+        <v>0.0</v>
+      </c>
+      <c r="F16" s="4" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="17" ht="375.0" customHeight="1">
+      <c r="A17" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="E17" s="4">
+        <v>0.0</v>
+      </c>
+      <c r="F17" s="4" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="18" ht="375.0" customHeight="1">
+      <c r="A18" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="E18" s="4">
+        <v>0.0</v>
+      </c>
+      <c r="F18" s="4" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="19" ht="375.0" customHeight="1">
+      <c r="A19" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="E19" s="4">
+        <v>-1.0</v>
+      </c>
+      <c r="F19" s="4" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="20" ht="375.0" customHeight="1">
+      <c r="A20" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="E20" s="4">
+        <v>-1.0</v>
+      </c>
+      <c r="F20" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="F1" s="3" t="s">
+    </row>
+    <row r="21" ht="375.0" customHeight="1">
+      <c r="A21" s="3" t="s">
         <v>101</v>
       </c>
+      <c r="B21" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="E21" s="4">
+        <v>0.0</v>
+      </c>
+      <c r="F21" s="4" t="s">
+        <v>105</v>
+      </c>
     </row>
-    <row r="2" spans="1:6" ht="409.6" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>7</v>
+    <row r="22" ht="375.0" customHeight="1">
+      <c r="A22" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="E22" s="4">
+        <v>-1.0</v>
+      </c>
+      <c r="F22" s="4" t="s">
+        <v>110</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="409.6" x14ac:dyDescent="0.2">
-      <c r="A3" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>11</v>
+    <row r="23" ht="375.0" customHeight="1">
+      <c r="A23" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="E23" s="4">
+        <v>0.0</v>
+      </c>
+      <c r="F23" s="4" t="s">
+        <v>115</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="409.6" x14ac:dyDescent="0.2">
-      <c r="A4" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>15</v>
+    <row r="24" ht="375.0" customHeight="1">
+      <c r="A24" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="D24" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="E24" s="4">
+        <v>0.0</v>
+      </c>
+      <c r="F24" s="4" t="s">
+        <v>120</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="409.6" x14ac:dyDescent="0.2">
-      <c r="A5" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="409.6" x14ac:dyDescent="0.2">
-      <c r="A6" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="409.6" x14ac:dyDescent="0.2">
-      <c r="A7" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" ht="409.6" x14ac:dyDescent="0.2">
-      <c r="A8" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" ht="409.6" x14ac:dyDescent="0.2">
-      <c r="A9" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" ht="409.6" x14ac:dyDescent="0.2">
-      <c r="A10" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" ht="409.6" x14ac:dyDescent="0.2">
-      <c r="A11" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" ht="409.6" x14ac:dyDescent="0.2">
-      <c r="A12" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" ht="409.6" x14ac:dyDescent="0.2">
-      <c r="A13" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" ht="409.6" x14ac:dyDescent="0.2">
-      <c r="A14" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" ht="409.6" x14ac:dyDescent="0.2">
-      <c r="A15" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" ht="409.6" x14ac:dyDescent="0.2">
-      <c r="A16" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="D16" s="2" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" ht="409.6" x14ac:dyDescent="0.2">
-      <c r="A17" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="D17" s="2" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" ht="409.6" x14ac:dyDescent="0.2">
-      <c r="A18" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="D18" s="2" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" ht="409.6" x14ac:dyDescent="0.2">
-      <c r="A19" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="C19" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="D19" s="2" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" ht="409.6" x14ac:dyDescent="0.2">
-      <c r="A20" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="C20" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="D20" s="2" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" ht="409.6" x14ac:dyDescent="0.2">
-      <c r="A21" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="B21" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="C21" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="D21" s="2" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" ht="409.6" x14ac:dyDescent="0.2">
-      <c r="A22" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="B22" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="C22" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="D22" s="2" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" ht="409.6" x14ac:dyDescent="0.2">
-      <c r="A23" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="B23" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="C23" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="D23" s="2" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" ht="409.6" x14ac:dyDescent="0.2">
-      <c r="A24" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="B24" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="C24" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="D24" s="2" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" ht="409.6" x14ac:dyDescent="0.2">
-      <c r="A25" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="B25" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="C25" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="D25" s="2" t="s">
-        <v>99</v>
+    <row r="25" ht="375.0" customHeight="1">
+      <c r="A25" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="D25" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="E25" s="4">
+        <v>0.0</v>
+      </c>
+      <c r="F25" s="4" t="s">
+        <v>125</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <printOptions/>
+  <pageMargins bottom="1.0" footer="0.0" header="0.0" left="0.75" right="0.75" top="1.0"/>
+  <pageSetup orientation="landscape"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>